<commit_message>
updated to work with groups
</commit_message>
<xml_diff>
--- a/Example Notebooks/custom_groups.xlsx
+++ b/Example Notebooks/custom_groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Dingwall\Documents\github\qub_canvas_helper\qub_canvas_helper\not for upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6397DB-426B-4182-8BE9-7AF2A9E12292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F66B29-0052-4F58-AF00-88813C0E10C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,21 +48,6 @@
     <t>Kate Winslet</t>
   </si>
   <si>
-    <t>Tuesday 10-1</t>
-  </si>
-  <si>
-    <t>Tuesday 2-5</t>
-  </si>
-  <si>
-    <t>Thursday 10-1</t>
-  </si>
-  <si>
-    <t>Thursday 2-5</t>
-  </si>
-  <si>
-    <t>Friday 2-5</t>
-  </si>
-  <si>
     <t>Lab 1</t>
   </si>
   <si>
@@ -76,13 +61,28 @@
   </si>
   <si>
     <t>Lab 5</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Group E</t>
+  </si>
+  <si>
+    <t>Group D</t>
+  </si>
+  <si>
+    <t>Group C</t>
+  </si>
+  <si>
+    <t>Group B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +95,14 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,11 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,128 +414,129 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C2" sqref="C2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1491</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1490</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1492</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1493</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -536,19 +546,19 @@
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>